<commit_message>
Addition of Autocorrelation Function
</commit_message>
<xml_diff>
--- a/crelox_data/2015_09_28_Control_S6_TS1.xlsx
+++ b/crelox_data/2015_09_28_Control_S6_TS1.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="480" yWindow="135" windowWidth="27795" windowHeight="15615" firstSheet="2" activeTab="3"/>
+    <workbookView xWindow="480" yWindow="135" windowWidth="27795" windowHeight="15615" firstSheet="2" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Stomatal Positions" sheetId="2" r:id="rId1"/>
@@ -2185,8 +2185,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D47"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2379,10 +2379,10 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" s="3">
-        <v>654.218017578125</v>
+        <v>720.218017578125</v>
       </c>
       <c r="B14" s="3">
-        <v>57.929000854492188</v>
+        <v>120.929000854492</v>
       </c>
       <c r="C14" s="3">
         <v>1324.1800537109375</v>
@@ -2862,8 +2862,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D108"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>

</xml_diff>